<commit_message>
Separated PixCel as a library
</commit_message>
<xml_diff>
--- a/Canvas.xlsx
+++ b/Canvas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pyExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFC2667-2E36-410C-A3FC-076CC7152ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19202A5A-CB1A-4EA3-8007-434DE93FD90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{B8F3985A-7ADF-4A5A-81D9-6BB996C2C047}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8F3985A-7ADF-4A5A-81D9-6BB996C2C047}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,74 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">#  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  #  #  #  #  #  #  #  #  #  #  #  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  #  #  #  #  #  #  #  #  #  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  #  #  #  #  #  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  _  _  _  #  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  #  #  #  #  #  #  #  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  _  _  _  #  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  _  _  _  #  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  #  #  #  #  #  #  #  _  _  #  _  _  _  _  _  _  _  _  _  _  _  _  #  </t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Adobe Caslon Pro"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Adobe Fan Heiti Std B"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,10 +70,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,170 +389,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759BACC1-49F2-477A-9455-5597E0854277}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A30"/>
+    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="139.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="2.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A21" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A26" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A28" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A29" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Made ASCII Bad Apple for MS-EXCEL
</commit_message>
<xml_diff>
--- a/Canvas.xlsx
+++ b/Canvas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pyExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19202A5A-CB1A-4EA3-8007-434DE93FD90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE2F6411-AF19-4BA5-AF94-835C84BB4F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8F3985A-7ADF-4A5A-81D9-6BB996C2C047}"/>
   </bookViews>
@@ -36,14 +36,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">_  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  #  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  _  </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -70,9 +85,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
   </cellXfs>
@@ -389,26 +405,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759BACC1-49F2-477A-9455-5597E0854277}">
-  <dimension ref="J1"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="21" zoomScaleNormal="21" workbookViewId="0">
+      <selection activeCell="AO64" sqref="AO64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="255.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>